<commit_message>
2º commit.He puesto los nombres
</commit_message>
<xml_diff>
--- a/Act01-Calificaciones.xlsx
+++ b/Act01-Calificaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AD_Presencial\_CURSO2223\UD01_ALUMNOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06790D02-C6B5-456E-962D-899E748F0990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D6ADA1-4411-41CD-8E99-F3EB50C4D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D7E05E17-3762-4250-88A1-AC4AB7DA7834}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Aplicación.  Gestion de ficheros</t>
   </si>
@@ -327,6 +327,18 @@
       </rPr>
       <t>Si  tiene subcarpetas no se eliminará.  Si contiene archivos se informará oportunamente y se pedirá confirmación si realmente se quiere seguir con la operación.</t>
     </r>
+  </si>
+  <si>
+    <t>Alba</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Laura</t>
   </si>
 </sst>
 </file>
@@ -775,10 +787,10 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,17 +800,25 @@
     <col min="3" max="15" width="7.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>

</xml_diff>